<commit_message>
ExcelSheet: bugfix with column index of head row not beginning with the first col index. RowIterator for dataRowIterator implemented for skipping empty rows.
</commit_message>
<xml_diff>
--- a/examples/Excel/Workbook-Test.xlsx
+++ b/examples/Excel/Workbook-Test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Java/merlin/examples/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839BA424-D07F-4F4B-A02A-50554CF1EC71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF15028B-2A7D-BB4F-9057-83E51005980A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="4000" windowWidth="27440" windowHeight="16560" xr2:uid="{ED2B2FD5-CDD0-364C-AACF-903ADCC1B665}"/>
+    <workbookView xWindow="5880" yWindow="4000" windowWidth="27440" windowHeight="16560" activeTab="1" xr2:uid="{ED2B2FD5-CDD0-364C-AACF-903ADCC1B665}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="empty rows" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>E-Mail</t>
   </si>
@@ -61,6 +62,9 @@
   </si>
   <si>
     <t>Kai Reinhard</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -435,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C8025C-81CF-FE49-8AF5-9844425213F6}">
   <dimension ref="A2:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,4 +512,80 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5BAF49-9516-1449-9F70-3A6E027F8FE5}">
+  <dimension ref="B4:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>48</v>
+      </c>
+      <c r="F5" s="3">
+        <v>43827</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>52</v>
+      </c>
+      <c r="F8" s="3">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{E73428B6-572D-4144-9FD2-865B3B8B787D}"/>
+    <hyperlink ref="C8" r:id="rId2" xr:uid="{DB968615-1EC4-6149-B506-FA14F9A15F7F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Testcase: ExcelSheet: test of customized columns for row emptiness check.
</commit_message>
<xml_diff>
--- a/examples/Excel/Workbook-Test.xlsx
+++ b/examples/Excel/Workbook-Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Java/merlin/examples/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF15028B-2A7D-BB4F-9057-83E51005980A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A22C570-0510-3F46-A399-17558A2E97BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5880" yWindow="4000" windowWidth="27440" windowHeight="16560" activeTab="1" xr2:uid="{ED2B2FD5-CDD0-364C-AACF-903ADCC1B665}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>E-Mail</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -516,10 +519,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5BAF49-9516-1449-9F70-3A6E027F8FE5}">
-  <dimension ref="B4:H11"/>
+  <dimension ref="B4:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,6 +583,16 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F12" s="3">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{E73428B6-572D-4144-9FD2-865B3B8B787D}"/>

</xml_diff>

<commit_message>
ExcelColumnDateValidator supports now Locale.
</commit_message>
<xml_diff>
--- a/examples/Excel/Workbook-Test.xlsx
+++ b/examples/Excel/Workbook-Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Java/merlin/examples/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77ED1E8D-C838-7244-817C-519FBD06B184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327177E1-D5A3-C349-97AC-DC53394095A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="4180" windowWidth="27440" windowHeight="16560" activeTab="2" xr2:uid="{ED2B2FD5-CDD0-364C-AACF-903ADCC1B665}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>E-Mail</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>2020-02-29 05:23</t>
+  </si>
+  <si>
+    <t>21. November 2020</t>
+  </si>
+  <si>
+    <t>21. November 2020 01:02</t>
+  </si>
+  <si>
+    <t>21. November 2020 1:2:17</t>
   </si>
 </sst>
 </file>
@@ -622,14 +631,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B602335-8DA3-2144-A625-64B6737AC603}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="26.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
   </cols>
@@ -674,6 +684,22 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
ImportHelper implemented for auto-filling beans from Excel rows. PoiHelper.getValue returns now LocalDateTime instead of java.util.Date at default.
</commit_message>
<xml_diff>
--- a/examples/Excel/Workbook-Test.xlsx
+++ b/examples/Excel/Workbook-Test.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Java/merlin/examples/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327177E1-D5A3-C349-97AC-DC53394095A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6287A24-984D-4245-BA0C-4FBB8C922F04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="4180" windowWidth="27440" windowHeight="16560" activeTab="2" xr2:uid="{ED2B2FD5-CDD0-364C-AACF-903ADCC1B665}"/>
+    <workbookView xWindow="920" yWindow="4180" windowWidth="27440" windowHeight="16560" activeTab="3" xr2:uid="{ED2B2FD5-CDD0-364C-AACF-903ADCC1B665}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
     <sheet name="empty rows" sheetId="2" r:id="rId2"/>
     <sheet name="dates" sheetId="3" r:id="rId3"/>
+    <sheet name="fillBean" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>E-Mail</t>
   </si>
@@ -93,12 +94,24 @@
   </si>
   <si>
     <t>21. November 2020 1:2:17</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>FloatValue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -145,12 +158,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -469,7 +484,7 @@
   <dimension ref="A2:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G4"/>
+      <selection activeCell="B2" sqref="B2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,11 +550,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{80B09543-9787-984C-9E44-7EC535047B08}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{E5CA27B6-2CD7-2946-A307-39CB4FA90237}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{0244001B-02C0-444A-9AE8-D481687399E9}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{E5CA27B6-2CD7-2946-A307-39CB4FA90237}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{80B09543-9787-984C-9E44-7EC535047B08}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -633,7 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B602335-8DA3-2144-A625-64B6737AC603}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -704,4 +720,97 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C142A3CB-1538-AE4E-96BC-F291254C6F6A}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>48</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43827</v>
+      </c>
+      <c r="E2" s="5">
+        <v>43831.996527777781</v>
+      </c>
+      <c r="F2" s="6">
+        <v>37.25</v>
+      </c>
+      <c r="G2">
+        <v>1.78</v>
+      </c>
+      <c r="H2">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>52</v>
+      </c>
+      <c r="D3" s="3">
+        <v>43830</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{E9C9A309-0569-A745-B32B-8800BF919969}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{A51DE0EA-03E0-AD4E-AE6F-AF7A29F5C61B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ImportHelper copies now numeric Excel values correctly to bean property.
</commit_message>
<xml_diff>
--- a/examples/Excel/Workbook-Test.xlsx
+++ b/examples/Excel/Workbook-Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Java/merlin/examples/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6287A24-984D-4245-BA0C-4FBB8C922F04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF62C37-9080-904A-AB71-00E4D6058ADC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="4180" windowWidth="27440" windowHeight="16560" activeTab="3" xr2:uid="{ED2B2FD5-CDD0-364C-AACF-903ADCC1B665}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>E-Mail</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>FloatValue</t>
+  </si>
+  <si>
+    <t>Text</t>
   </si>
 </sst>
 </file>
@@ -110,7 +113,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -165,7 +168,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -724,10 +727,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C142A3CB-1538-AE4E-96BC-F291254C6F6A}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -739,7 +742,7 @@
     <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -764,8 +767,11 @@
       <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -790,8 +796,11 @@
       <c r="H2">
         <v>1.27</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
ExcelRow.copyAndInsert: shift only if not at the end. ExcelSheet: getEmptyRows < lastRowNum.
</commit_message>
<xml_diff>
--- a/examples/Excel/Workbook-Test.xlsx
+++ b/examples/Excel/Workbook-Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Java/merlin/examples/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70705C1-21E2-5141-81F9-A10B01057D39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097EAC15-A2DB-1A41-BE99-A9294EDDC262}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="4320" windowWidth="27440" windowHeight="16560" activeTab="4" xr2:uid="{ED2B2FD5-CDD0-364C-AACF-903ADCC1B665}"/>
+    <workbookView xWindow="1420" yWindow="11920" windowWidth="27440" windowHeight="16560" activeTab="4" xr2:uid="{ED2B2FD5-CDD0-364C-AACF-903ADCC1B665}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,12 @@
     <sheet name="fillBean" sheetId="4" r:id="rId4"/>
     <sheet name="Row-actions" sheetId="5" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Icons">#REF!</definedName>
     <definedName name="Item_Types">#REF!</definedName>
     <definedName name="KNX_Channel_Types">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -237,12 +234,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -259,29 +256,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Validator-Test"/>
-      <sheetName val="Clean-Test"/>
-      <sheetName val="Config"/>
-      <sheetName val="Validator-Mass-Test"/>
-      <sheetName val="Empty-sheet"/>
-      <sheetName val="Empty-sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -926,7 +900,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,81 +920,81 @@
     </row>
     <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>0.05</v>
       </c>
       <c r="E3" s="6">
         <v>17</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="10"/>
       <c r="J3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>0.05</v>
       </c>
       <c r="E4" s="6">
         <v>17</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="10"/>
       <c r="J4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>0.05</v>
       </c>
       <c r="E5" s="6">
         <v>17</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="10"/>
       <c r="J5" t="s">
         <v>31</v>
       </c>
@@ -1028,54 +1002,54 @@
     <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>0.05</v>
       </c>
       <c r="E8" s="6">
         <v>17</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="10"/>
       <c r="J8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>0.05</v>
       </c>
       <c r="E9" s="6">
         <v>17</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="10"/>
       <c r="J9" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Bugfix in copyAndInsert. copyCellsFrom(srcRow) supports now merged regions (inside the current row).
</commit_message>
<xml_diff>
--- a/examples/Excel/Workbook-Test.xlsx
+++ b/examples/Excel/Workbook-Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/workspace/Java/merlin/examples/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097EAC15-A2DB-1A41-BE99-A9294EDDC262}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0673780-BFE8-E841-B38F-30E5ED27202A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="11920" windowWidth="27440" windowHeight="16560" activeTab="4" xr2:uid="{ED2B2FD5-CDD0-364C-AACF-903ADCC1B665}"/>
+    <workbookView xWindow="1420" yWindow="11920" windowWidth="27440" windowHeight="16560" xr2:uid="{ED2B2FD5-CDD0-364C-AACF-903ADCC1B665}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="Item_Types">#REF!</definedName>
     <definedName name="KNX_Channel_Types">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
   <si>
     <t>E-Mail</t>
   </si>
@@ -138,6 +138,21 @@
   </si>
   <si>
     <t>last</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Box 1</t>
+  </si>
+  <si>
+    <t>red, underline 1</t>
+  </si>
+  <si>
+    <t>combined 1</t>
+  </si>
+  <si>
+    <t>last 1</t>
   </si>
 </sst>
 </file>
@@ -226,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -240,6 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -555,11 +571,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C8025C-81CF-FE49-8AF5-9844425213F6}">
-  <dimension ref="A2:G4"/>
+  <dimension ref="A2:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -567,7 +581,7 @@
     <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -588,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -608,7 +622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -621,8 +635,16 @@
       <c r="E4" s="3">
         <v>43830</v>
       </c>
+      <c r="F4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F4:H4"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{E5CA27B6-2CD7-2946-A307-39CB4FA90237}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{0244001B-02C0-444A-9AE8-D481687399E9}"/>
@@ -899,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED62C72-134A-3C4B-B232-A6253F6D8449}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -908,7 +930,7 @@
     <col min="7" max="7" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -916,6 +938,28 @@
     <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E2" s="6">
+        <v>15</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1055,7 +1099,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>

</xml_diff>